<commit_message>
Ben hat was mit den Playerstats vorbereitet - schau gern mal drübber :)
</commit_message>
<xml_diff>
--- a/2023-bis-2025-Spielerstatistiken-R.xlsx
+++ b/2023-bis-2025-Spielerstatistiken-R.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Documents\MEK 2024-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0E2FBF-4FD4-4E89-A1B9-7CAE5B64497D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73D0B33-99C8-4D98-AACF-B0D70046965F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Sharapa, Vasily</t>
   </si>
   <si>
@@ -369,10 +366,13 @@
     <t>s2324</t>
   </si>
   <si>
-    <t>sgp2324</t>
-  </si>
-  <si>
     <t>eff2324</t>
+  </si>
+  <si>
+    <t>spg2324</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -726,9 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -738,81 +736,81 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>96</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>97</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>98</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>99</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>100</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>101</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>102</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>104</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>105</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>106</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>107</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>108</v>
-      </c>
-      <c r="V1" t="s">
-        <v>109</v>
       </c>
       <c r="W1" t="s">
         <v>110</v>
       </c>
       <c r="X1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -892,7 +890,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -972,7 +970,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1052,7 +1050,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1132,7 +1130,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1212,7 +1210,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1292,7 +1290,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1372,7 +1370,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1452,7 +1450,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1532,7 +1530,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1612,7 +1610,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1692,7 +1690,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1772,7 +1770,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1852,7 +1850,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1932,7 +1930,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2012,7 +2010,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2092,7 +2090,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2172,7 +2170,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2252,7 +2250,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2332,7 +2330,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2412,7 +2410,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2492,7 +2490,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2572,7 +2570,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2652,7 +2650,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2732,7 +2730,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2812,7 +2810,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2892,7 +2890,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2972,7 +2970,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3052,7 +3050,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -3132,7 +3130,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3212,7 +3210,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3292,7 +3290,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3372,7 +3370,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3452,7 +3450,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -3532,7 +3530,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3612,7 +3610,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3692,7 +3690,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -3772,7 +3770,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -3852,7 +3850,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -3939,7 +3937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3949,244 +3949,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
         <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
         <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
         <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4194,21 +4194,21 @@
         <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>